<commit_message>
Things seem to be in order
</commit_message>
<xml_diff>
--- a/UCSO-2019/Updatable Files/Tests.xlsx
+++ b/UCSO-2019/Updatable Files/Tests.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Internal number</t>
   </si>
@@ -149,6 +149,54 @@
   </si>
   <si>
     <t>ERC 201B/247</t>
+  </si>
+  <si>
+    <t>Crime Busters</t>
+  </si>
+  <si>
+    <t>Game On</t>
+  </si>
+  <si>
+    <t>Heredity</t>
+  </si>
+  <si>
+    <t>Meteorology</t>
+  </si>
+  <si>
+    <t>Potions &amp; Poisons</t>
+  </si>
+  <si>
+    <t>Road Scholar</t>
+  </si>
+  <si>
+    <t>Solar System</t>
+  </si>
+  <si>
+    <t>Cobb 430</t>
+  </si>
+  <si>
+    <t>Stuart 101</t>
+  </si>
+  <si>
+    <t>CSIL 2</t>
+  </si>
+  <si>
+    <t>Hinds 184</t>
+  </si>
+  <si>
+    <t>Ida Noyes East Lounge</t>
+  </si>
+  <si>
+    <t>KPTC 103</t>
+  </si>
+  <si>
+    <t>BSLC 313</t>
+  </si>
+  <si>
+    <t>BSLC 346</t>
+  </si>
+  <si>
+    <t>Cobb 402/409</t>
   </si>
 </sst>
 </file>
@@ -633,10 +681,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -973,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1669,160 +1719,442 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="A20" s="5">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5">
+        <v>50</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>9</v>
+      </c>
+      <c r="G20" s="4">
+        <v>10</v>
+      </c>
+      <c r="H20" s="4">
+        <v>11</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="A21" s="5">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5">
+        <v>50</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>12</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>9</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="A22" s="5">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="5">
+        <v>50</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4">
+        <v>11</v>
+      </c>
+      <c r="H22" s="4">
+        <v>12</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="A23" s="5">
+        <v>31</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="5">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>8</v>
+      </c>
+      <c r="G23" s="4">
+        <v>8</v>
+      </c>
+      <c r="H23" s="4">
+        <v>8</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="A24" s="5">
+        <v>32</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5">
+        <v>50</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>9</v>
+      </c>
+      <c r="H24" s="4">
+        <v>10</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="A25" s="5">
+        <v>35</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <v>9</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="A26" s="5">
+        <v>36</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5">
+        <v>50</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>10</v>
+      </c>
+      <c r="G26" s="4">
+        <v>11</v>
+      </c>
+      <c r="H26" s="4">
+        <v>12</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="A27" s="5">
+        <v>37</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="5">
+        <v>50</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <v>9</v>
+      </c>
+      <c r="H27" s="4">
+        <v>10</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="A28" s="5">
+        <v>38</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5">
+        <v>50</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>10</v>
+      </c>
+      <c r="G28" s="4">
+        <v>11</v>
+      </c>
+      <c r="H28" s="4">
+        <v>12</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="A29" s="5">
+        <v>39</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="5">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>11</v>
+      </c>
+      <c r="G29" s="4">
+        <v>12</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="A30" s="5">
+        <v>41</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="5">
+        <v>50</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>9</v>
+      </c>
+      <c r="G30" s="4">
+        <v>10</v>
+      </c>
+      <c r="H30" s="4">
+        <v>11</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="A31" s="5">
+        <v>42</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="5">
+        <v>50</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>9</v>
+      </c>
+      <c r="G31" s="4">
+        <v>10</v>
+      </c>
+      <c r="H31" s="4">
+        <v>11</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="2"/>
+      <c r="A32" s="5">
+        <v>44</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="5">
+        <v>50</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="4">
+        <v>10</v>
+      </c>
+      <c r="G32" s="4">
+        <v>11</v>
+      </c>
+      <c r="H32" s="4">
+        <v>12</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="3:13">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+    <row r="33" spans="1:13">
+      <c r="A33" s="5">
+        <v>46</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="5">
+        <v>50</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>11</v>
+      </c>
+      <c r="G33" s="4">
+        <v>12</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1</v>
+      </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="3:13">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+    <row r="34" spans="1:13">
+      <c r="A34" s="5">
+        <v>47</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5">
+        <v>50</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F34" s="4">
+        <v>11</v>
+      </c>
+      <c r="G34" s="4">
+        <v>12</v>
+      </c>
+      <c r="H34" s="4">
+        <v>1</v>
+      </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="3:13">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+    <row r="35" spans="1:13">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
@@ -1830,12 +2162,14 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
     </row>
-    <row r="36" spans="3:13">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+    <row r="36" spans="1:13">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -1843,149 +2177,180 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="3:13">
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="G37" s="1"/>
+    <row r="37" spans="1:13">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="3:13">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="G38" s="1"/>
+    <row r="38" spans="1:13">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="3:13">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="G39" s="1"/>
+    <row r="39" spans="1:13">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="3:13">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="G40" s="1"/>
+    <row r="40" spans="1:13">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="3:13">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="G41" s="1"/>
+    <row r="41" spans="1:13">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="3:13">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="G42" s="1"/>
+    <row r="42" spans="1:13">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="3:13">
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="G43" s="1"/>
+    <row r="43" spans="1:13">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="3:13">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="G44" s="1"/>
+    <row r="44" spans="1:13">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="3:13">
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="G45" s="1"/>
+    <row r="45" spans="1:13">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="3:13">
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="G46" s="1"/>
+    <row r="46" spans="1:13">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="3:13">
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="G47" s="1"/>
+    <row r="47" spans="1:13">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="3:13">
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="G48" s="1"/>
+    <row r="48" spans="1:13">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="3:10">
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="G49" s="1"/>
+    <row r="49" spans="4:10">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="3:10">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="G50" s="1"/>
+    <row r="50" spans="4:10">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="3:10">
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="G51" s="1"/>
+    <row r="51" spans="4:10">
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="3:10">
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+    <row r="52" spans="4:10">
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="4:10">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="4:10">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="C26:J57">
-    <sortCondition ref="C26"/>
+  <sortState ref="A32:G54">
+    <sortCondition ref="E32:E54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>